<commit_message>
Updated Sprint Task Sheet
</commit_message>
<xml_diff>
--- a/Reports/Team Enigma - Sprint Task Sheet.xlsx
+++ b/Reports/Team Enigma - Sprint Task Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brinda/sjsu/CMPE202/project/fa21-202-team-enigma/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8593615-3CF1-8149-8FD4-913F50C55B78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34CB4187-996A-274D-9720-D9091D5DCED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,13 +232,13 @@
     <t>Total Available Hours During Sprint:</t>
   </si>
   <si>
-    <t>Code Design and Analysis for adding functionality - Booster points Meteor</t>
-  </si>
-  <si>
     <t>Feature Implementation for adding functionality - Booster points Meteor</t>
   </si>
   <si>
-    <t>Testing for functionality - Booster points Meteor</t>
+    <t>Code Design and Analysis for adding functionality - Booster points Meteor and Learn Git</t>
+  </si>
+  <si>
+    <t>Testing for functionality - Booster points Meteor and review feature- Reverse Words</t>
   </si>
 </sst>
 </file>
@@ -969,79 +969,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="29"/>
                 <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>58</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>58</c:v>
+                <c:pt idx="5">
+                  <c:v>57</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>54</c:v>
+                <c:pt idx="6">
+                  <c:v>55</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>51</c:v>
+                <c:pt idx="7">
+                  <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>46</c:v>
+                <c:pt idx="8">
+                  <c:v>53</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="9">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>45</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>43</c:v>
+                <c:pt idx="11">
+                  <c:v>42</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="12">
                   <c:v>41</c:v>
                 </c:pt>
-                <c:pt idx="8">
-                  <c:v>41</c:v>
+                <c:pt idx="13">
+                  <c:v>23</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>35</c:v>
+                <c:pt idx="14">
+                  <c:v>21</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>33</c:v>
+                <c:pt idx="15">
+                  <c:v>19</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>30</c:v>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
                 </c:pt>
-                <c:pt idx="12">
-                  <c:v>29</c:v>
+                <c:pt idx="17">
+                  <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="18">
                   <c:v>11</c:v>
                 </c:pt>
-                <c:pt idx="14">
-                  <c:v>9</c:v>
+                <c:pt idx="19">
+                  <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="20">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="22">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>1</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0</c:v>
@@ -1794,7 +1794,7 @@
   <dimension ref="A1:AG999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:AF5"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2169,103 +2169,103 @@
       </c>
       <c r="E5" s="10">
         <f>SUM(E6:E35)</f>
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="F5" s="10">
         <f t="shared" ref="F5:AF5" si="1">SUM(F6:F35)</f>
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="G5" s="10">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="H5" s="10">
         <f t="shared" si="1"/>
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="I5" s="10">
         <f t="shared" si="1"/>
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="J5" s="10">
         <f t="shared" si="1"/>
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="K5" s="10">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="L5" s="10">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="M5" s="10">
         <f t="shared" si="1"/>
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="N5" s="10">
         <f t="shared" si="1"/>
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="O5" s="10">
         <f t="shared" si="1"/>
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="P5" s="10">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="Q5" s="10">
         <f t="shared" si="1"/>
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="R5" s="10">
         <f t="shared" si="1"/>
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="S5" s="10">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="T5" s="10">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="U5" s="10">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="V5" s="10">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="W5" s="10">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="X5" s="10">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="Y5" s="10">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="Z5" s="10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="AA5" s="10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="AB5" s="10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AC5" s="10">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AD5" s="10">
         <f t="shared" si="1"/>
@@ -2960,7 +2960,7 @@
     <row r="17" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="27"/>
       <c r="B17" s="12" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C17" s="13" t="s">
         <v>42</v>
@@ -3238,7 +3238,7 @@
     <row r="22" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A22" s="27"/>
       <c r="B22" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C22" s="13" t="s">
         <v>42</v>
@@ -3496,34 +3496,90 @@
       <c r="D27" s="13">
         <v>4</v>
       </c>
-      <c r="E27" s="18"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="18"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="16"/>
-      <c r="O27" s="16"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="16"/>
-      <c r="R27" s="16"/>
-      <c r="S27" s="18"/>
-      <c r="T27" s="18"/>
-      <c r="U27" s="18"/>
-      <c r="V27" s="18"/>
-      <c r="W27" s="18"/>
-      <c r="X27" s="18"/>
-      <c r="Y27" s="18"/>
-      <c r="Z27" s="16"/>
-      <c r="AA27" s="16"/>
-      <c r="AB27" s="16"/>
-      <c r="AC27" s="16"/>
-      <c r="AD27" s="16"/>
-      <c r="AE27" s="16"/>
-      <c r="AF27" s="16"/>
+      <c r="E27" s="18">
+        <v>4</v>
+      </c>
+      <c r="F27" s="18">
+        <v>4</v>
+      </c>
+      <c r="G27" s="18">
+        <v>4</v>
+      </c>
+      <c r="H27" s="18">
+        <v>4</v>
+      </c>
+      <c r="I27" s="18">
+        <v>4</v>
+      </c>
+      <c r="J27" s="18">
+        <v>4</v>
+      </c>
+      <c r="K27" s="18">
+        <v>4</v>
+      </c>
+      <c r="L27" s="16">
+        <v>4</v>
+      </c>
+      <c r="M27" s="16">
+        <v>4</v>
+      </c>
+      <c r="N27" s="16">
+        <v>4</v>
+      </c>
+      <c r="O27" s="16">
+        <v>4</v>
+      </c>
+      <c r="P27" s="16">
+        <v>4</v>
+      </c>
+      <c r="Q27" s="16">
+        <v>4</v>
+      </c>
+      <c r="R27" s="16">
+        <v>4</v>
+      </c>
+      <c r="S27" s="18">
+        <v>4</v>
+      </c>
+      <c r="T27" s="18">
+        <v>4</v>
+      </c>
+      <c r="U27" s="18">
+        <v>4</v>
+      </c>
+      <c r="V27" s="18">
+        <v>3</v>
+      </c>
+      <c r="W27" s="18">
+        <v>1</v>
+      </c>
+      <c r="X27" s="18">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="18">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="16">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="16">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="16">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="16">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="16">
+        <v>0</v>
+      </c>
+      <c r="AE27" s="16">
+        <v>0</v>
+      </c>
+      <c r="AF27" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A28" s="27"/>
@@ -3686,34 +3742,90 @@
       <c r="D32" s="13">
         <v>8</v>
       </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="16"/>
-      <c r="O32" s="16"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
-      <c r="S32" s="18"/>
-      <c r="T32" s="18"/>
-      <c r="U32" s="18"/>
-      <c r="V32" s="18"/>
-      <c r="W32" s="18"/>
-      <c r="X32" s="18"/>
-      <c r="Y32" s="18"/>
-      <c r="Z32" s="16"/>
-      <c r="AA32" s="16"/>
-      <c r="AB32" s="16"/>
-      <c r="AC32" s="16"/>
-      <c r="AD32" s="16"/>
-      <c r="AE32" s="16"/>
-      <c r="AF32" s="16"/>
+      <c r="E32" s="18">
+        <v>8</v>
+      </c>
+      <c r="F32" s="18">
+        <v>8</v>
+      </c>
+      <c r="G32" s="18">
+        <v>8</v>
+      </c>
+      <c r="H32" s="18">
+        <v>8</v>
+      </c>
+      <c r="I32" s="18">
+        <v>8</v>
+      </c>
+      <c r="J32" s="18">
+        <v>8</v>
+      </c>
+      <c r="K32" s="18">
+        <v>8</v>
+      </c>
+      <c r="L32" s="16">
+        <v>8</v>
+      </c>
+      <c r="M32" s="16">
+        <v>8</v>
+      </c>
+      <c r="N32" s="16">
+        <v>8</v>
+      </c>
+      <c r="O32" s="16">
+        <v>8</v>
+      </c>
+      <c r="P32" s="16">
+        <v>8</v>
+      </c>
+      <c r="Q32" s="16">
+        <v>8</v>
+      </c>
+      <c r="R32" s="16">
+        <v>8</v>
+      </c>
+      <c r="S32" s="18">
+        <v>8</v>
+      </c>
+      <c r="T32" s="18">
+        <v>8</v>
+      </c>
+      <c r="U32" s="18">
+        <v>8</v>
+      </c>
+      <c r="V32" s="18">
+        <v>8</v>
+      </c>
+      <c r="W32" s="18">
+        <v>8</v>
+      </c>
+      <c r="X32" s="18">
+        <v>8</v>
+      </c>
+      <c r="Y32" s="18">
+        <v>8</v>
+      </c>
+      <c r="Z32" s="16">
+        <v>6</v>
+      </c>
+      <c r="AA32" s="16">
+        <v>5</v>
+      </c>
+      <c r="AB32" s="16">
+        <v>4</v>
+      </c>
+      <c r="AC32" s="16">
+        <v>2</v>
+      </c>
+      <c r="AD32" s="16">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="16">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="16">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:32" ht="13" x14ac:dyDescent="0.15">
       <c r="A33" s="27"/>

</xml_diff>

<commit_message>
Update Sprint Task Sheet
</commit_message>
<xml_diff>
--- a/Reports/Team Enigma - Sprint Task Sheet.xlsx
+++ b/Reports/Team Enigma - Sprint Task Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sai07/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brinda/sjsu/CMPE202/project/fa21-202-team-enigma/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27F437C-0014-9E46-88D0-34CEEF92C84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A0540E-CB04-EF4C-90DE-23CC19208B1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="71">
   <si>
     <t>Week #1 (10 hrs / week)</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Testing for</t>
   </si>
   <si>
-    <t>Testing for functionality - Booster points Meteor and review feature- Reverse Words</t>
-  </si>
-  <si>
     <t>Testing for functionality - Masked words</t>
   </si>
   <si>
@@ -243,6 +240,12 @@
   <si>
     <t>Total Available Hours During Sprint:</t>
   </si>
+  <si>
+    <t>Github Administration - manage branches of peers and Architecture diagram, User Story Video and Demo Video</t>
+  </si>
+  <si>
+    <t>Testing for functionality - Booster points Meteor and review features - Reverse Words, Masked Words, Pause Play buttons</t>
+  </si>
 </sst>
 </file>
 
@@ -251,7 +254,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m&quot;/&quot;d"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -290,6 +293,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -547,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -634,17 +643,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -654,13 +660,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1769,8 +1779,8 @@
   </sheetPr>
   <dimension ref="A1:AG1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="AD27" sqref="AD27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1788,51 +1798,51 @@
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
       <c r="D1" s="3"/>
-      <c r="E1" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
-      <c r="H1" s="40"/>
-      <c r="I1" s="40"/>
-      <c r="J1" s="40"/>
-      <c r="K1" s="41"/>
-      <c r="L1" s="42" t="s">
+      <c r="E1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="40"/>
+      <c r="L1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="40"/>
-      <c r="N1" s="40"/>
-      <c r="O1" s="40"/>
-      <c r="P1" s="40"/>
-      <c r="Q1" s="40"/>
-      <c r="R1" s="41"/>
-      <c r="S1" s="39" t="s">
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="40"/>
-      <c r="U1" s="40"/>
-      <c r="V1" s="40"/>
-      <c r="W1" s="40"/>
-      <c r="X1" s="40"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="42" t="s">
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39"/>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="40"/>
-      <c r="AB1" s="40"/>
-      <c r="AC1" s="40"/>
-      <c r="AD1" s="40"/>
-      <c r="AE1" s="40"/>
-      <c r="AF1" s="43"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="39"/>
+      <c r="AE1" s="39"/>
+      <c r="AF1" s="42"/>
     </row>
     <row r="2" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="43" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="43" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="44" t="s">
@@ -1924,9 +1934,9 @@
       </c>
     </row>
     <row r="3" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
       <c r="D3" s="45"/>
       <c r="E3" s="7">
         <v>41944</v>
@@ -2015,9 +2025,9 @@
       <c r="AG3" s="8"/>
     </row>
     <row r="4" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="9">
         <v>200</v>
       </c>
@@ -2138,9 +2148,9 @@
       </c>
     </row>
     <row r="5" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="36"/>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
       <c r="D5" s="9">
         <v>200</v>
       </c>
@@ -2261,7 +2271,7 @@
       </c>
     </row>
     <row r="6" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="46" t="s">
         <v>38</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -2359,7 +2369,7 @@
       </c>
     </row>
     <row r="7" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="35"/>
+      <c r="A7" s="36"/>
       <c r="B7" s="12" t="s">
         <v>41</v>
       </c>
@@ -2455,7 +2465,7 @@
       </c>
     </row>
     <row r="8" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="35"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="12" t="s">
         <v>43</v>
       </c>
@@ -2493,7 +2503,7 @@
       <c r="AF8" s="18"/>
     </row>
     <row r="9" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="35"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="12" t="s">
         <v>45</v>
       </c>
@@ -2589,7 +2599,7 @@
       </c>
     </row>
     <row r="10" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="35"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="12" t="s">
         <v>47</v>
       </c>
@@ -2685,7 +2695,7 @@
       </c>
     </row>
     <row r="11" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="35"/>
+      <c r="A11" s="36"/>
       <c r="B11" s="12" t="s">
         <v>49</v>
       </c>
@@ -2781,7 +2791,7 @@
       </c>
     </row>
     <row r="12" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="35"/>
+      <c r="A12" s="36"/>
       <c r="B12" s="12" t="s">
         <v>50</v>
       </c>
@@ -2877,7 +2887,7 @@
       </c>
     </row>
     <row r="13" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="35"/>
+      <c r="A13" s="36"/>
       <c r="B13" s="12" t="s">
         <v>51</v>
       </c>
@@ -2915,7 +2925,7 @@
       <c r="AF13" s="18"/>
     </row>
     <row r="14" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="35"/>
+      <c r="A14" s="36"/>
       <c r="B14" s="12" t="s">
         <v>52</v>
       </c>
@@ -3011,7 +3021,7 @@
       </c>
     </row>
     <row r="15" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="36"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="12" t="s">
         <v>53</v>
       </c>
@@ -3107,7 +3117,7 @@
       </c>
     </row>
     <row r="16" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="35" t="s">
         <v>54</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -3167,7 +3177,7 @@
       <c r="AF16" s="18"/>
     </row>
     <row r="17" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="35"/>
+      <c r="A17" s="36"/>
       <c r="B17" s="12" t="s">
         <v>56</v>
       </c>
@@ -3263,7 +3273,7 @@
       </c>
     </row>
     <row r="18" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="35"/>
+      <c r="A18" s="36"/>
       <c r="B18" s="12" t="s">
         <v>57</v>
       </c>
@@ -3301,7 +3311,7 @@
       <c r="AF18" s="18"/>
     </row>
     <row r="19" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="35"/>
+      <c r="A19" s="36"/>
       <c r="B19" s="12" t="s">
         <v>57</v>
       </c>
@@ -3397,7 +3407,7 @@
       </c>
     </row>
     <row r="20" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="36"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="12" t="s">
         <v>57</v>
       </c>
@@ -3493,7 +3503,7 @@
       </c>
     </row>
     <row r="21" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="38" t="s">
+      <c r="A21" s="35" t="s">
         <v>54</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -3561,7 +3571,7 @@
       <c r="AF21" s="18"/>
     </row>
     <row r="22" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="35"/>
+      <c r="A22" s="36"/>
       <c r="B22" s="12" t="s">
         <v>59</v>
       </c>
@@ -3657,7 +3667,7 @@
       </c>
     </row>
     <row r="23" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="35"/>
+      <c r="A23" s="36"/>
       <c r="B23" s="12" t="s">
         <v>60</v>
       </c>
@@ -3695,7 +3705,7 @@
       <c r="AF23" s="18"/>
     </row>
     <row r="24" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="35"/>
+      <c r="A24" s="36"/>
       <c r="B24" s="12" t="s">
         <v>60</v>
       </c>
@@ -3791,7 +3801,7 @@
       </c>
     </row>
     <row r="25" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="36"/>
+      <c r="A25" s="37"/>
       <c r="B25" s="12" t="s">
         <v>60</v>
       </c>
@@ -3846,7 +3856,7 @@
       <c r="S25" s="15">
         <v>0</v>
       </c>
-      <c r="T25" s="46">
+      <c r="T25" s="34">
         <v>0</v>
       </c>
       <c r="U25" s="15">
@@ -3887,7 +3897,7 @@
       </c>
     </row>
     <row r="26" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="38" t="s">
+      <c r="A26" s="35" t="s">
         <v>61</v>
       </c>
       <c r="B26" s="12" t="s">
@@ -3927,9 +3937,9 @@
       <c r="AF26" s="18"/>
     </row>
     <row r="27" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="35"/>
-      <c r="B27" s="12" t="s">
-        <v>63</v>
+      <c r="A27" s="36"/>
+      <c r="B27" s="47" t="s">
+        <v>70</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>42</v>
@@ -4023,7 +4033,7 @@
       </c>
     </row>
     <row r="28" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="35"/>
+      <c r="A28" s="36"/>
       <c r="B28" s="12" t="s">
         <v>62</v>
       </c>
@@ -4061,9 +4071,9 @@
       <c r="AF28" s="18"/>
     </row>
     <row r="29" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="35"/>
+      <c r="A29" s="36"/>
       <c r="B29" s="29" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C29" s="13" t="s">
         <v>46</v>
@@ -4157,7 +4167,7 @@
       </c>
     </row>
     <row r="30" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="36"/>
+      <c r="A30" s="37"/>
       <c r="B30" s="12" t="s">
         <v>62</v>
       </c>
@@ -4253,8 +4263,8 @@
       </c>
     </row>
     <row r="31" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="38" t="s">
-        <v>65</v>
+      <c r="A31" s="35" t="s">
+        <v>64</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="13" t="s">
@@ -4291,8 +4301,10 @@
       <c r="AF31" s="18"/>
     </row>
     <row r="32" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="35"/>
-      <c r="B32" s="12"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="C32" s="13" t="s">
         <v>42</v>
       </c>
@@ -4385,7 +4397,7 @@
       </c>
     </row>
     <row r="33" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="35"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="12"/>
       <c r="C33" s="13" t="s">
         <v>44</v>
@@ -4421,7 +4433,7 @@
       <c r="AF33" s="18"/>
     </row>
     <row r="34" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="35"/>
+      <c r="A34" s="36"/>
       <c r="B34" s="12"/>
       <c r="C34" s="13" t="s">
         <v>46</v>
@@ -4457,7 +4469,7 @@
       <c r="AF34" s="18"/>
     </row>
     <row r="35" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="36"/>
+      <c r="A35" s="37"/>
       <c r="B35" s="12"/>
       <c r="C35" s="13" t="s">
         <v>48</v>
@@ -4534,10 +4546,10 @@
     </row>
     <row r="38" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="B38" s="30" t="s">
         <v>66</v>
-      </c>
-      <c r="B38" s="30" t="s">
-        <v>67</v>
       </c>
       <c r="C38" s="30"/>
       <c r="D38" s="30"/>
@@ -4563,7 +4575,7 @@
         <v>42</v>
       </c>
       <c r="B39" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C39" s="30"/>
       <c r="D39" s="30"/>
@@ -4586,10 +4598,10 @@
     </row>
     <row r="40" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C40" s="30"/>
       <c r="D40" s="30"/>
@@ -4615,7 +4627,7 @@
         <v>44</v>
       </c>
       <c r="B41" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C41" s="30"/>
       <c r="D41" s="30"/>
@@ -4641,7 +4653,7 @@
         <v>46</v>
       </c>
       <c r="B42" s="30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C42" s="30"/>
       <c r="D42" s="30"/>
@@ -4664,7 +4676,7 @@
     </row>
     <row r="43" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B43" s="32">
         <f>4*50</f>

</xml_diff>